<commit_message>
Research on Existing Technologies and Comparision
</commit_message>
<xml_diff>
--- a/Documentation/Complete Project Timeline.xlsx
+++ b/Documentation/Complete Project Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5849fbde5c4cf694/Desktop/College - Uni/Uni Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="115" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2C637E6-1CF1-4588-8835-D9ABDCF82D20}"/>
+  <xr:revisionPtr revIDLastSave="132" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0AADF432-16BF-4AE2-8B46-E0090A3D7BFE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{43229390-D9E6-4EBD-A715-EF6E60A7C3EE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -132,6 +132,27 @@
   </si>
   <si>
     <t>First Version of the Background Paragraph</t>
+  </si>
+  <si>
+    <t>08.10.2022</t>
+  </si>
+  <si>
+    <t>Outline of Specifications and Terminology: Chord, Riff, Monophone/Polyphone</t>
+  </si>
+  <si>
+    <t>Wiring Experiment</t>
+  </si>
+  <si>
+    <t>Create an Arduino 4X4 Numpad</t>
+  </si>
+  <si>
+    <t>09.10.2022</t>
+  </si>
+  <si>
+    <t>Research</t>
+  </si>
+  <si>
+    <t>Existing Technologies, Guitar Hero, MI Digital Guitar, RockSmith and their specifications and Comparision Section</t>
   </si>
 </sst>
 </file>
@@ -507,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B349D5-7FEC-4BA2-A4F4-AEC45E6B72AD}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,7 +782,55 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D15" s="4">
+      <c r="A15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15">
+        <v>60</v>
+      </c>
+      <c r="E15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16">
+        <v>190</v>
+      </c>
+      <c r="E16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D19" s="4">
         <f>SUM(D2:D7) / 60</f>
         <v>8.9166666666666661</v>
       </c>

</xml_diff>

<commit_message>
Project Aim and Objectives 1st Sketch
</commit_message>
<xml_diff>
--- a/Documentation/Complete Project Timeline.xlsx
+++ b/Documentation/Complete Project Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5849fbde5c4cf694/Desktop/College - Uni/Uni Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="132" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0AADF432-16BF-4AE2-8B46-E0090A3D7BFE}"/>
+  <xr:revisionPtr revIDLastSave="165" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05BF8BDA-CDC9-4E80-9B4A-B0AF76B598E8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{43229390-D9E6-4EBD-A715-EF6E60A7C3EE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
   <si>
     <t>Date</t>
   </si>
@@ -140,9 +140,6 @@
     <t>Outline of Specifications and Terminology: Chord, Riff, Monophone/Polyphone</t>
   </si>
   <si>
-    <t>Wiring Experiment</t>
-  </si>
-  <si>
     <t>Create an Arduino 4X4 Numpad</t>
   </si>
   <si>
@@ -153,6 +150,39 @@
   </si>
   <si>
     <t>Existing Technologies, Guitar Hero, MI Digital Guitar, RockSmith and their specifications and Comparision Section</t>
+  </si>
+  <si>
+    <t>Research Gap, Aim and Objectives Paragraph, Literature Review: Sketch Strum vs Strumbar Task Plan</t>
+  </si>
+  <si>
+    <t>TBA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arduino Experiment 4X4 Matrix </t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Tutorial</t>
+  </si>
+  <si>
+    <t>Experiment</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>Project Aim and Objectives</t>
+  </si>
+  <si>
+    <t>Existing Technologies</t>
+  </si>
+  <si>
+    <t>Minutes</t>
+  </si>
+  <si>
+    <t>Hours</t>
   </si>
 </sst>
 </file>
@@ -182,12 +212,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -202,11 +238,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -214,6 +247,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B349D5-7FEC-4BA2-A4F4-AEC45E6B72AD}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,300 +578,385 @@
     <col min="1" max="1" width="12.42578125" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="30.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="155.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="155.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>0.93055555555555547</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2">
         <v>60</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>0.62152777777777779</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3">
         <v>90</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>0.79513888888888884</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4">
         <v>95</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>0.62152777777777779</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5">
         <v>80</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>0.66666666666666663</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6">
         <v>80</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>0.88194444444444453</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="D7">
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7">
         <v>130</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>0.97222222222222221</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
       </c>
-      <c r="D8">
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8">
         <v>95</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>0.76041666666666663</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="D9">
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9">
         <v>80</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>0.875</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
       </c>
-      <c r="D10">
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10">
         <v>100</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>0.77083333333333337</v>
       </c>
       <c r="C11" t="s">
         <v>23</v>
       </c>
-      <c r="D11">
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11">
         <v>120</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>0.96875</v>
       </c>
       <c r="C12" t="s">
         <v>26</v>
       </c>
-      <c r="D12">
+      <c r="D12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12">
         <v>240</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>0.14583333333333334</v>
       </c>
       <c r="C13" t="s">
         <v>28</v>
       </c>
-      <c r="D13">
+      <c r="D13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13">
         <v>140</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>0.3888888888888889</v>
       </c>
       <c r="C14" t="s">
         <v>28</v>
       </c>
-      <c r="D14">
+      <c r="D14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14">
         <v>50</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>0.66666666666666663</v>
       </c>
       <c r="C15" t="s">
         <v>28</v>
       </c>
-      <c r="D15">
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15">
         <v>60</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="3">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="E16">
+        <v>190</v>
+      </c>
+      <c r="F16" t="s">
         <v>37</v>
       </c>
-      <c r="D16">
-        <v>190</v>
-      </c>
-      <c r="E16" t="s">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="2">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17">
+        <v>80</v>
+      </c>
+      <c r="F17" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="3"/>
-      <c r="C17" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="2"/>
+      <c r="C18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" t="s">
         <v>34</v>
       </c>
-      <c r="E17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="3"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D19" s="4">
-        <f>SUM(D2:D7) / 60</f>
-        <v>8.9166666666666661</v>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D20" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="3">
+        <f>SUM(E2:E19)</f>
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D21" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="3">
+        <f>E20 / 60</f>
+        <v>28.166666666666668</v>
       </c>
     </row>
   </sheetData>

</xml_diff>